<commit_message>
Add reply comment method
</commit_message>
<xml_diff>
--- a/Inititial methods list.xlsx
+++ b/Inititial methods list.xlsx
@@ -59,9 +59,6 @@
     <t>Rating hospital and clinic</t>
   </si>
   <si>
-    <t>Comment about any hospital or clinic</t>
-  </si>
-  <si>
     <t>Feedback about information of the system</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>View statistics about their business</t>
+  </si>
+  <si>
+    <t>Comment / Reply comment about any hospital or clinic</t>
   </si>
 </sst>
 </file>
@@ -726,7 +726,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -740,7 +740,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -755,7 +755,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -768,7 +768,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -792,7 +792,7 @@
     </row>
     <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2" t="s">
@@ -810,7 +810,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -824,7 +824,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -839,7 +839,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -852,7 +852,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -867,7 +867,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -881,7 +881,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -894,7 +894,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -918,11 +918,11 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -936,7 +936,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -950,7 +950,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -965,7 +965,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -978,7 +978,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
       <c r="D30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -992,7 +992,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1007,7 +1007,7 @@
       <c r="C32" s="6"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>

</xml_diff>

<commit_message>
Add method approve feedback
</commit_message>
<xml_diff>
--- a/Inititial methods list.xlsx
+++ b/Inititial methods list.xlsx
@@ -104,9 +104,6 @@
     <t>(Active or deactive members)</t>
   </si>
   <si>
-    <t>View users' feedback</t>
-  </si>
-  <si>
     <t>Import hospitals and clinics data</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Comment / Reply comment about any hospital or clinic</t>
+  </si>
+  <si>
+    <t>View and approve users' feedback</t>
   </si>
 </sst>
 </file>
@@ -726,7 +726,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -894,7 +894,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -978,7 +978,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
       <c r="D30" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -992,7 +992,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1007,7 +1007,7 @@
       <c r="C32" s="6"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>

</xml_diff>

<commit_message>
Rename Premium User to Hospital User. Remove approve appointment method of Hospital User. Add view statistics method for Administrator.
</commit_message>
<xml_diff>
--- a/Inititial methods list.xlsx
+++ b/Inititial methods list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14895" windowHeight="3420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Role</t>
   </si>
@@ -47,9 +47,6 @@
     <t>(Desription, comments, rating)</t>
   </si>
   <si>
-    <t>Normal member</t>
-  </si>
-  <si>
     <t>Have all priorities that provided for Guest</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Make appointment online</t>
   </si>
   <si>
-    <t>Premium member</t>
-  </si>
-  <si>
     <t>Login with provided system's account</t>
   </si>
   <si>
@@ -117,13 +111,19 @@
   </si>
   <si>
     <t>View and approve users' feedback</t>
+  </si>
+  <si>
+    <t>Normal User</t>
+  </si>
+  <si>
+    <t>Hospital User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +155,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -262,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -275,6 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K32"/>
+  <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -581,32 +589,32 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="13"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
@@ -680,11 +688,11 @@
     </row>
     <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -698,7 +706,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -712,7 +720,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -726,7 +734,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -740,7 +748,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -755,7 +763,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -768,7 +776,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -792,11 +800,11 @@
     </row>
     <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -810,7 +818,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -824,7 +832,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -839,7 +847,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -852,7 +860,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -867,7 +875,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -881,7 +889,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -894,7 +902,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -918,17 +926,17 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="I26" s="12"/>
       <c r="J26" s="2"/>
       <c r="K26" s="3"/>
     </row>
@@ -936,7 +944,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -950,7 +958,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -965,7 +973,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -978,7 +986,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
       <c r="D30" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -992,7 +1000,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1002,19 +1010,33 @@
       <c r="J31" s="2"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="4"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="6"/>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>